<commit_message>
Fix more typos etc
</commit_message>
<xml_diff>
--- a/Statement of Applicability - ISO27001:2022.xlsx
+++ b/Statement of Applicability - ISO27001:2022.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26426"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9D71180D-625D-4ECA-95E7-4E0C61D19404}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E24ED838-3065-48D4-ADDD-5F3007D6DE6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Statement of Applicability" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="328">
   <si>
     <t>Control</t>
   </si>
@@ -52,6 +52,9 @@
     <t>Responsibility</t>
   </si>
   <si>
+    <t>Remarks</t>
+  </si>
+  <si>
     <t>5. Organizational controls</t>
   </si>
   <si>
@@ -73,7 +76,7 @@
     <t>Information security roles and responsibilities</t>
   </si>
   <si>
-    <t>Information security roles and responsibilities shall be defined and allocated Control according to the organization needs.</t>
+    <t>Information security roles and responsibilities shall be defined and allocated according to the organization needs.</t>
   </si>
   <si>
     <t>A. 5.3</t>
@@ -379,7 +382,7 @@
     <t>Compliance with policies, rules and standards for information security</t>
   </si>
   <si>
-    <t>Comliance with the organization's information security policy, topic-specific policies rules and standards shall be regularly reviewed.</t>
+    <t>Compliance with the organization's information security policy, topic-specific policies rules and standards shall be regularly reviewed.</t>
   </si>
   <si>
     <t>A. 5.37</t>
@@ -400,7 +403,7 @@
     <t>Screening</t>
   </si>
   <si>
-    <t>Background verification checks on all candidates to become personnel shall be carried out prior to joining the organization and on an ongoing basis taking into consideration applicable laws, regulations and ethics and be proportional to the business requirements, the classification of</t>
+    <t>Background verification checks on all candidates to become personnel shall be carried out prior to joining the organization and on an ongoing basis taking into consideration applicable laws, regulations and ethics and be proportional to the business requirements, the classification of the information to be accessed and the perceived risks.</t>
   </si>
   <si>
     <t>A. 6.2</t>
@@ -409,7 +412,7 @@
     <t>Terms and conditions of employment</t>
   </si>
   <si>
-    <t>the information to be accessed and the perceived risks.</t>
+    <t>The employment contractual agreements shall state the personnel’s and the organization’s responsibilities for information security.</t>
   </si>
   <si>
     <t>A. 6.3</t>
@@ -454,7 +457,7 @@
     <t>Remote working</t>
   </si>
   <si>
-    <t>relevant interested parties.</t>
+    <t>Security measures shall be implemented when personnel are working remotely to protect information accessed, processed or stored outside the organization’s premises.</t>
   </si>
   <si>
     <t>A. 6.8</t>
@@ -992,6 +995,12 @@
   </si>
   <si>
     <t>Chief Technology Officer</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>Board</t>
   </si>
   <si>
     <t>AS</t>
@@ -1010,7 +1019,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1040,13 +1049,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1068,13 +1070,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1594,51 +1595,54 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A7:H107"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="G70" sqref="G70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="57.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="230.5703125" customWidth="1"/>
+    <col min="3" max="3" width="110.7109375" customWidth="1"/>
     <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="30.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="7" spans="1:8" ht="15" customHeight="1">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="G7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H7" s="3"/>
+      <c r="H7" s="3" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="8" spans="1:8" ht="15" customHeight="1">
-      <c r="A8" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
+      <c r="A8" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -1646,1948 +1650,1930 @@
     </row>
     <row r="9" spans="1:8" ht="15" customHeight="1">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15" customHeight="1">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15" customHeight="1">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="15" customHeight="1">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="15" customHeight="1">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D13" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E13" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G13" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="15" customHeight="1">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D14" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E14" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G14" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="15" customHeight="1">
       <c r="A15" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D15" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E15" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G15" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="15" customHeight="1">
       <c r="A16" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D16" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E16" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G16" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="15" customHeight="1">
       <c r="A17" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D17" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E17" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G17" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="15" customHeight="1">
       <c r="A18" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D18" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E18" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G18" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="15" customHeight="1">
       <c r="A19" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D19" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E19" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G19" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="15" customHeight="1">
       <c r="A20" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D20" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E20" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G20" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="15" customHeight="1">
       <c r="A21" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D21" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E21" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G21" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="15" customHeight="1">
       <c r="A22" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D22" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E22" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G22" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="15" customHeight="1">
       <c r="A23" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D23" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E23" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G23" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="15" customHeight="1">
       <c r="A24" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D24" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E24" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G24" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="15" customHeight="1">
       <c r="A25" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D25" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E25" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G25" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="15" customHeight="1">
       <c r="A26" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D26" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E26" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G26" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="15" customHeight="1">
       <c r="A27" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D27" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E27" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G27" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="15" customHeight="1">
       <c r="A28" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D28" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E28" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G28" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="15" customHeight="1">
       <c r="A29" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D29" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E29" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G29" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="15" customHeight="1">
       <c r="A30" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D30" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E30" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G30" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="15" customHeight="1">
       <c r="A31" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D31" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E31" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G31" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="15" customHeight="1">
       <c r="A32" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D32" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E32" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G32" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="15" customHeight="1">
       <c r="A33" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D33" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E33" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G33" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="15" customHeight="1">
       <c r="A34" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D34" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E34" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G34" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="15" customHeight="1">
       <c r="A35" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D35" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E35" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G35" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="15" customHeight="1">
       <c r="A36" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D36" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E36" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G36" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="15" customHeight="1">
       <c r="A37" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D37" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E37" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G37" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="15" customHeight="1">
       <c r="A38" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D38" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E38" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G38" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="15" customHeight="1">
       <c r="A39" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D39" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E39" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G39" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="15" customHeight="1">
       <c r="A40" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D40" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E40" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G40" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="15" customHeight="1">
       <c r="A41" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D41" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E41" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G41" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="15" customHeight="1">
       <c r="A42" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D42" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E42" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G42" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="15" customHeight="1">
       <c r="A43" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D43" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E43" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G43" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="15" customHeight="1">
       <c r="A44" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D44" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E44" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G44" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="15" customHeight="1">
       <c r="A45" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D45" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E45" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G45" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="15" customHeight="1">
-      <c r="A46" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="B46" s="6"/>
-      <c r="C46" s="6"/>
+      <c r="A46" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B46" s="5"/>
+      <c r="C46" s="5"/>
     </row>
     <row r="47" spans="1:7" ht="15" customHeight="1">
       <c r="A47" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B47" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C47" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D47" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E47" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G47" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="15" customHeight="1">
       <c r="A48" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B48" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C48" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D48" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E48" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G48" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="15" customHeight="1">
       <c r="A49" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B49" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C49" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D49" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E49" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G49" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="15" customHeight="1">
       <c r="A50" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B50" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C50" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D50" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E50" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G50" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="15" customHeight="1">
       <c r="A51" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B51" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C51" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D51" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E51" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G51" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="15" customHeight="1">
       <c r="A52" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B52" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C52" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D52" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E52" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G52" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="15" customHeight="1">
       <c r="A53" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B53" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C53" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D53" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E53" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G53" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="15" customHeight="1">
       <c r="A54" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B54" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C54" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D54" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E54" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G54" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="15" customHeight="1">
-      <c r="A55" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="B55" s="7"/>
-      <c r="C55" s="7"/>
-      <c r="D55" t="s">
-        <v>11</v>
-      </c>
-      <c r="E55" t="s">
-        <v>11</v>
-      </c>
-      <c r="G55" t="s">
-        <v>11</v>
-      </c>
+      <c r="A55" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="B55" s="6"/>
+      <c r="C55" s="6"/>
     </row>
     <row r="56" spans="1:7" ht="15" customHeight="1">
       <c r="A56" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B56" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C56" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D56" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E56" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G56" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="15" customHeight="1">
       <c r="A57" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B57" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C57" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D57" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E57" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G57" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="58" spans="1:7" ht="15" customHeight="1">
       <c r="A58" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B58" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C58" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D58" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E58" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G58" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="15" customHeight="1">
       <c r="A59" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B59" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C59" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D59" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E59" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G59" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="60" spans="1:7" ht="15" customHeight="1">
       <c r="A60" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B60" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C60" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D60" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E60" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G60" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="15" customHeight="1">
       <c r="A61" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B61" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C61" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D61" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E61" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G61" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="62" spans="1:7" ht="15" customHeight="1">
       <c r="A62" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B62" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C62" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D62" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E62" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G62" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="63" spans="1:7" ht="15" customHeight="1">
       <c r="A63" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B63" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C63" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D63" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E63" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G63" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="64" spans="1:7" ht="15" customHeight="1">
       <c r="A64" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B64" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C64" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D64" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E64" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G64" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="65" spans="1:7" ht="15" customHeight="1">
       <c r="A65" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B65" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C65" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D65" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E65" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G65" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="66" spans="1:7" ht="15" customHeight="1">
       <c r="A66" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B66" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C66" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D66" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E66" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G66" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="15" customHeight="1">
       <c r="A67" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B67" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C67" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D67" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E67" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G67" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="68" spans="1:7" ht="15" customHeight="1">
       <c r="A68" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B68" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C68" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D68" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E68" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G68" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="69" spans="1:7" ht="15" customHeight="1">
       <c r="A69" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B69" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C69" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D69" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E69" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G69" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="15" customHeight="1">
-      <c r="A70" s="7" t="s">
-        <v>188</v>
-      </c>
-      <c r="B70" s="7"/>
-      <c r="C70" s="7"/>
-      <c r="D70" t="s">
-        <v>11</v>
-      </c>
-      <c r="E70" t="s">
-        <v>11</v>
-      </c>
-      <c r="G70" t="s">
-        <v>11</v>
-      </c>
+      <c r="A70" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="B70" s="6"/>
+      <c r="C70" s="6"/>
     </row>
     <row r="71" spans="1:7" ht="15" customHeight="1">
       <c r="A71" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B71" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C71" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D71" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E71" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G71" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="15" customHeight="1">
       <c r="A72" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B72" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C72" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D72" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E72" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G72" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="15" customHeight="1">
       <c r="A73" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B73" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C73" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="D73" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E73" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G73" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="74" spans="1:7" ht="15" customHeight="1">
       <c r="A74" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B74" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C74" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="D74" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E74" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G74" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="75" spans="1:7" ht="15" customHeight="1">
       <c r="A75" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B75" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C75" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="D75" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E75" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G75" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="76" spans="1:7" ht="15" customHeight="1">
       <c r="A76" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B76" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C76" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D76" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E76" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G76" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="77" spans="1:7" ht="15" customHeight="1">
       <c r="A77" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B77" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C77" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D77" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E77" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G77" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="78" spans="1:7" ht="15" customHeight="1">
       <c r="A78" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B78" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C78" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="D78" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E78" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G78" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="79" spans="1:7" ht="15" customHeight="1">
       <c r="A79" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B79" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C79" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D79" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E79" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G79" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="80" spans="1:7" ht="15" customHeight="1">
       <c r="A80" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B80" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C80" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="D80" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E80" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G80" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="81" spans="1:7" ht="15" customHeight="1">
       <c r="A81" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B81" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C81" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="D81" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E81" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G81" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="82" spans="1:7" ht="15" customHeight="1">
       <c r="A82" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B82" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C82" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="D82" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E82" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G82" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="83" spans="1:7" ht="15" customHeight="1">
       <c r="A83" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B83" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C83" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="D83" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E83" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G83" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="84" spans="1:7" ht="15" customHeight="1">
       <c r="A84" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B84" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C84" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="D84" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E84" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G84" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="85" spans="1:7" ht="15" customHeight="1">
       <c r="A85" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B85" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C85" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D85" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E85" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G85" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="86" spans="1:7" ht="15" customHeight="1">
       <c r="A86" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B86" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="C86" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="D86" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E86" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G86" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="87" spans="1:7" ht="15" customHeight="1">
       <c r="A87" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B87" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C87" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="D87" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E87" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G87" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="88" spans="1:7" ht="15" customHeight="1">
       <c r="A88" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B88" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="C88" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="D88" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E88" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G88" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="89" spans="1:7" ht="15" customHeight="1">
       <c r="A89" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B89" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C89" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="D89" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E89" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G89" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="90" spans="1:7" ht="15" customHeight="1">
       <c r="A90" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B90" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C90" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="D90" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E90" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G90" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="91" spans="1:7" ht="15" customHeight="1">
       <c r="A91" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B91" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C91" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="D91" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E91" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G91" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="92" spans="1:7" ht="15" customHeight="1">
       <c r="A92" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B92" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="C92" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="D92" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E92" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G92" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="93" spans="1:7" ht="15" customHeight="1">
       <c r="A93" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="B93" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="C93" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="D93" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E93" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G93" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="94" spans="1:7" ht="15" customHeight="1">
       <c r="A94" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="B94" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="C94" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="D94" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E94" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G94" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="95" spans="1:7" ht="15" customHeight="1">
       <c r="A95" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B95" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C95" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="D95" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E95" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G95" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="96" spans="1:7" ht="15" customHeight="1">
       <c r="A96" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B96" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="C96" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="D96" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E96" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G96" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="97" spans="1:7" ht="15" customHeight="1">
       <c r="A97" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B97" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="C97" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="D97" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E97" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G97" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="98" spans="1:7" ht="15" customHeight="1">
       <c r="A98" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B98" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C98" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="D98" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E98" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G98" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="99" spans="1:7" ht="15" customHeight="1">
       <c r="A99" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B99" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C99" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="D99" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E99" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G99" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="100" spans="1:7" ht="15" customHeight="1">
       <c r="A100" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="B100" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="C100" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="D100" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E100" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G100" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="101" spans="1:7" ht="15" customHeight="1">
       <c r="A101" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="B101" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="C101" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="D101" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E101" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G101" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="102" spans="1:7" ht="15" customHeight="1">
       <c r="A102" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="B102" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="C102" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D102" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E102" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G102" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="103" spans="1:7" ht="15" customHeight="1">
       <c r="A103" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="B103" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="C103" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D103" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E103" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G103" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="104" spans="1:7" ht="15" customHeight="1">
       <c r="A104" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B104" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="C104" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="D104" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E104" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G104" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="105" spans="1:7" ht="15" customHeight="1">
-      <c r="A105" s="7" t="s">
-        <v>291</v>
-      </c>
-      <c r="B105" s="7"/>
-      <c r="C105" s="7"/>
+      <c r="A105" s="6" t="s">
+        <v>292</v>
+      </c>
+      <c r="B105" s="6"/>
+      <c r="C105" s="6"/>
     </row>
     <row r="106" spans="1:7" ht="15" customHeight="1">
       <c r="A106" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B106" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="C106" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="D106" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E106" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G106" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="107" spans="1:7" ht="15" customHeight="1">
       <c r="A107" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="B107" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C107" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="D107" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E107" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G107" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -3661,9 +3647,9 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{BC103332-0192-4525-84E8-E64F50943881}">
           <x14:formula1>
-            <xm:f>Legend!$B$20:$B$24</xm:f>
+            <xm:f>Legend!$B$20:$B$25</xm:f>
           </x14:formula1>
-          <xm:sqref>G9:G45 G47:G104 G106:G107</xm:sqref>
+          <xm:sqref>G9:G45 G106:G107 G47:G104</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3673,9 +3659,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{606BA237-E2BB-4547-95BD-710D4376385C}">
-  <dimension ref="B3:C24"/>
+  <dimension ref="B3:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
@@ -3695,42 +3681,42 @@
     </row>
     <row r="4" spans="2:3">
       <c r="B4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
     </row>
     <row r="5" spans="2:3">
       <c r="B5" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="C5" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="6" spans="2:3">
       <c r="B6" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="C6" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
     </row>
     <row r="7" spans="2:3">
       <c r="B7" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="C7" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
     </row>
     <row r="8" spans="2:3">
       <c r="B8" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="C8" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="10" spans="2:3">
@@ -3743,58 +3729,58 @@
     </row>
     <row r="11" spans="2:3">
       <c r="B11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C11" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
     </row>
     <row r="12" spans="2:3">
       <c r="B12" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="C12" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="13" spans="2:3">
       <c r="B13" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="C13" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="14" spans="2:3">
       <c r="B14" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="C14" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="15" spans="2:3">
       <c r="B15" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="C15" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row r="16" spans="2:3">
       <c r="B16" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C16" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="17" spans="2:3">
       <c r="B17" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="C17" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="19" spans="2:3">
@@ -3807,42 +3793,50 @@
     </row>
     <row r="20" spans="2:3">
       <c r="B20" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C20" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
     </row>
     <row r="21" spans="2:3">
       <c r="B21" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="C21" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="22" spans="2:3">
       <c r="B22" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="C22" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
     </row>
     <row r="23" spans="2:3">
       <c r="B23" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="C23" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="24" spans="2:3">
       <c r="B24" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="C24" t="s">
-        <v>324</v>
+        <v>325</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3">
+      <c r="B25" t="s">
+        <v>326</v>
+      </c>
+      <c r="C25" t="s">
+        <v>327</v>
       </c>
     </row>
   </sheetData>

</xml_diff>